<commit_message>
IMPLEMENTED CSV->ScriptableObjects Workflow for Items
Ahhh, this automation feels just ***swell***. Now, I have become Prometheus and gifted mankind (also me) the boon of fire (automating writing endless data).
Thank goodness this works! Now I can do the same thing with CharacterUnits to create friends, enemies, allies, all the same from centralized CSV files that determine all of the pertinent data. This is so cool!!!

:camel:
</commit_message>
<xml_diff>
--- a/Assets/Documents/Items.xlsx
+++ b/Assets/Documents/Items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahcedeno/Documents/GitHub/2D-TRPG-Idea/Assets/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69294F1A-48B6-F045-ABE8-A4E609D737CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF192257-E209-8545-B776-0BCE2D0B9A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{206ABD45-FC92-784F-A300-25B6BF6B1218}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14160" xr2:uid="{206ABD45-FC92-784F-A300-25B6BF6B1218}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -164,11 +164,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +487,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,13 +625,16 @@
         <v>125</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
       </c>
       <c r="K5" t="s">
         <v>18</v>
@@ -658,13 +662,16 @@
         <v>100</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2</v>
       </c>
       <c r="K6" t="s">
         <v>19</v>
@@ -692,13 +699,16 @@
         <v>275</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
       </c>
       <c r="K7" t="s">
         <v>19</v>
@@ -782,7 +792,13 @@
         <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
+      <c r="I10" s="4">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -804,7 +820,13 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3</v>
+      </c>
+      <c r="J11" s="3">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>